<commit_message>
Added export from scriptable object to .csv
</commit_message>
<xml_diff>
--- a/Assets/CSV/CardDatabase.xlsx
+++ b/Assets/CSV/CardDatabase.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ORade\Documents\Unity\Stadsbouer\Stadsbouer\Assets\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38177CC-CC49-4D21-A0C9-1C67E18F63D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E04546-044B-4E09-973A-94B44A2BEB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="card_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>Card Name</t>
   </si>
@@ -200,6 +201,18 @@
   </si>
   <si>
     <t>TradeCenter.fbx</t>
+  </si>
+  <si>
+    <t>Ability?</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -342,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +533,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -683,8 +708,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1064,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,5 +1556,118 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2450FDE1-BFE3-44FE-BEEE-3FC32C694E9E}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E2E96D5-F154-4F58-9E04-7B53C5870331}">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA1D2DB6-308A-493A-B611-D9FF1F035CCE}">
+          <x14:formula1>
+            <xm:f>Lists!$C$2:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0538AA07-FE62-4392-9300-35139DC9416D}">
+          <x14:formula1>
+            <xm:f>Lists!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7738CB1-B70D-49EA-BEC2-913653138FA2}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>